<commit_message>
Chipped away at car inventory, did some brainstorming
I did a little bit of tedious code for the car inventory, and I did a bit of brainstorming too.
</commit_message>
<xml_diff>
--- a/RPG Items.xlsx
+++ b/RPG Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ranged Weapons" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="451">
   <si>
     <t>Name</t>
   </si>
@@ -973,9 +973,6 @@
     <t>various animal and mutated animal types that players hunt</t>
   </si>
   <si>
-    <t>Things like deer, rabbits, quails, ducks, but also mutated things like jackalopes</t>
-  </si>
-  <si>
     <t>hunting background</t>
   </si>
   <si>
@@ -1307,6 +1304,81 @@
   </si>
   <si>
     <t>a desperate person with less health and speed</t>
+  </si>
+  <si>
+    <t>guitar</t>
+  </si>
+  <si>
+    <t>ukelele</t>
+  </si>
+  <si>
+    <t>banjo</t>
+  </si>
+  <si>
+    <t>gourd banjo</t>
+  </si>
+  <si>
+    <t>cello</t>
+  </si>
+  <si>
+    <t>hermonica</t>
+  </si>
+  <si>
+    <t>blowing jug</t>
+  </si>
+  <si>
+    <t>can play music minigame, can equip to play music while exploring</t>
+  </si>
+  <si>
+    <t>bass</t>
+  </si>
+  <si>
+    <t>Healthy scavenger</t>
+  </si>
+  <si>
+    <t>a desparate person who normally wouldn't attack a player unless they think they can take them and get stuff- if they have low health or exceptionally flashy items</t>
+  </si>
+  <si>
+    <t>Confederate</t>
+  </si>
+  <si>
+    <t>believes the south will rise again</t>
+  </si>
+  <si>
+    <t>Neonazi</t>
+  </si>
+  <si>
+    <t>white supremacist, allied with confederates</t>
+  </si>
+  <si>
+    <t>Communist</t>
+  </si>
+  <si>
+    <t>soldier for cummunist faction</t>
+  </si>
+  <si>
+    <t>BoPossum</t>
+  </si>
+  <si>
+    <t>big ol' possum</t>
+  </si>
+  <si>
+    <t>Horse and Cart</t>
+  </si>
+  <si>
+    <t>tamborine</t>
+  </si>
+  <si>
+    <t>Things like deer, squirrels, rabbits, quails, ducks, but also mutated things like jackalopes</t>
+  </si>
+  <si>
+    <t>Illness</t>
+  </si>
+  <si>
+    <t>walkie-talkie</t>
+  </si>
+  <si>
+    <t>Extends the range players cal walk away from each other</t>
   </si>
 </sst>
 </file>
@@ -1732,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3419,7 +3491,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N2"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3675,16 +3747,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D9"/>
+  <dimension ref="A2:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.1640625" customWidth="1"/>
+    <col min="2" max="2" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
@@ -3773,6 +3845,116 @@
         <v>75</v>
       </c>
       <c r="C9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>426</v>
+      </c>
+      <c r="B10" t="s">
+        <v>433</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>427</v>
+      </c>
+      <c r="B11" t="s">
+        <v>433</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>428</v>
+      </c>
+      <c r="B12" t="s">
+        <v>433</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>429</v>
+      </c>
+      <c r="B13" t="s">
+        <v>433</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>430</v>
+      </c>
+      <c r="B14" t="s">
+        <v>433</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>434</v>
+      </c>
+      <c r="B15" t="s">
+        <v>433</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>446</v>
+      </c>
+      <c r="B16" t="s">
+        <v>433</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>431</v>
+      </c>
+      <c r="B17" t="s">
+        <v>433</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>432</v>
+      </c>
+      <c r="B18" t="s">
+        <v>433</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>449</v>
+      </c>
+      <c r="B19" t="s">
+        <v>450</v>
+      </c>
+      <c r="C19" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3791,7 +3973,7 @@
   <dimension ref="A2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3897,7 +4079,7 @@
         <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>448</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -3920,7 +4102,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>448</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -3950,10 +4132,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4287,79 +4469,134 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B26" t="s">
         <v>103</v>
       </c>
       <c r="E26" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B27" t="s">
         <v>106</v>
       </c>
       <c r="E27" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B28" t="s">
         <v>106</v>
       </c>
       <c r="E28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B29" t="s">
         <v>108</v>
       </c>
       <c r="E29" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B30" t="s">
         <v>103</v>
       </c>
       <c r="E30" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B31" t="s">
         <v>103</v>
       </c>
       <c r="E31" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B32" t="s">
         <v>103</v>
       </c>
       <c r="E32" t="s">
-        <v>426</v>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>435</v>
+      </c>
+      <c r="B33" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>437</v>
+      </c>
+      <c r="B34" t="s">
+        <v>103</v>
+      </c>
+      <c r="E34" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>439</v>
+      </c>
+      <c r="B35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>441</v>
+      </c>
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>443</v>
+      </c>
+      <c r="B37" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" t="s">
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -4376,8 +4613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4561,7 +4798,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B11" t="s">
         <v>278</v>
@@ -4570,15 +4807,15 @@
         <v>143</v>
       </c>
       <c r="D11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B12" t="s">
         <v>278</v>
@@ -4587,10 +4824,10 @@
         <v>143</v>
       </c>
       <c r="D12" t="s">
+        <v>352</v>
+      </c>
+      <c r="E12" t="s">
         <v>353</v>
-      </c>
-      <c r="E12" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -4655,10 +4892,10 @@
         <v>142</v>
       </c>
       <c r="D16" t="s">
+        <v>332</v>
+      </c>
+      <c r="E16" t="s">
         <v>333</v>
-      </c>
-      <c r="E16" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -4714,7 +4951,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B20" t="s">
         <v>313</v>
@@ -4726,12 +4963,12 @@
         <v>314</v>
       </c>
       <c r="E20" t="s">
-        <v>315</v>
+        <v>447</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B21" t="s">
         <v>313</v>
@@ -4740,15 +4977,15 @@
         <v>142</v>
       </c>
       <c r="D21" t="s">
+        <v>316</v>
+      </c>
+      <c r="E21" t="s">
         <v>317</v>
-      </c>
-      <c r="E21" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B22" t="s">
         <v>313</v>
@@ -4757,15 +4994,15 @@
         <v>143</v>
       </c>
       <c r="D22" t="s">
+        <v>323</v>
+      </c>
+      <c r="E22" t="s">
         <v>324</v>
-      </c>
-      <c r="E22" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B23" t="s">
         <v>313</v>
@@ -4774,58 +5011,58 @@
         <v>142</v>
       </c>
       <c r="D23" t="s">
+        <v>321</v>
+      </c>
+      <c r="E23" t="s">
         <v>322</v>
-      </c>
-      <c r="E23" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C24" t="s">
         <v>143</v>
       </c>
       <c r="D24" t="s">
+        <v>334</v>
+      </c>
+      <c r="E24" t="s">
         <v>335</v>
-      </c>
-      <c r="E24" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C25" t="s">
         <v>143</v>
       </c>
       <c r="D25" t="s">
+        <v>336</v>
+      </c>
+      <c r="E25" t="s">
         <v>337</v>
-      </c>
-      <c r="E25" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B26" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C26" t="s">
         <v>142</v>
       </c>
       <c r="D26" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E26" t="s">
         <v>27</v>
@@ -4833,50 +5070,50 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C27" t="s">
         <v>142</v>
       </c>
       <c r="D27" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
+        <v>329</v>
+      </c>
+      <c r="B28" t="s">
         <v>330</v>
-      </c>
-      <c r="B28" t="s">
-        <v>331</v>
       </c>
       <c r="C28" t="s">
         <v>143</v>
       </c>
       <c r="D28" t="s">
+        <v>344</v>
+      </c>
+      <c r="E28" t="s">
         <v>345</v>
-      </c>
-      <c r="E28" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C29" t="s">
         <v>142</v>
       </c>
       <c r="D29" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E29" t="s">
         <v>27</v>
@@ -4884,118 +5121,118 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C30" t="s">
         <v>142</v>
       </c>
       <c r="D30" t="s">
+        <v>347</v>
+      </c>
+      <c r="E30" t="s">
         <v>348</v>
-      </c>
-      <c r="E30" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
+        <v>350</v>
+      </c>
+      <c r="B31" t="s">
         <v>351</v>
       </c>
-      <c r="B31" t="s">
-        <v>352</v>
-      </c>
       <c r="C31" t="s">
         <v>142</v>
       </c>
       <c r="D31" t="s">
+        <v>354</v>
+      </c>
+      <c r="E31" t="s">
         <v>355</v>
-      </c>
-      <c r="E31" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B32" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C32" t="s">
         <v>143</v>
       </c>
       <c r="D32" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E32" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
+        <v>358</v>
+      </c>
+      <c r="B33" t="s">
+        <v>351</v>
+      </c>
+      <c r="C33" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" t="s">
         <v>359</v>
       </c>
-      <c r="B33" t="s">
-        <v>352</v>
-      </c>
-      <c r="C33" t="s">
-        <v>142</v>
-      </c>
-      <c r="D33" t="s">
-        <v>360</v>
-      </c>
       <c r="E33" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
+        <v>377</v>
+      </c>
+      <c r="B34" t="s">
         <v>378</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" t="s">
         <v>379</v>
       </c>
-      <c r="C34" t="s">
-        <v>142</v>
-      </c>
-      <c r="D34" t="s">
-        <v>380</v>
-      </c>
       <c r="E34" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C35" t="s">
         <v>143</v>
       </c>
       <c r="D35" t="s">
+        <v>382</v>
+      </c>
+      <c r="E35" t="s">
         <v>383</v>
-      </c>
-      <c r="E35" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
+        <v>385</v>
+      </c>
+      <c r="B36" t="s">
         <v>386</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" t="s">
         <v>387</v>
-      </c>
-      <c r="C36" t="s">
-        <v>142</v>
-      </c>
-      <c r="D36" t="s">
-        <v>388</v>
       </c>
       <c r="E36" t="s">
         <v>27</v>
@@ -5003,138 +5240,138 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B37" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C37" t="s">
         <v>143</v>
       </c>
       <c r="D37" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E37" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B38" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C38" t="s">
         <v>143</v>
       </c>
       <c r="D38" t="s">
+        <v>392</v>
+      </c>
+      <c r="E38" t="s">
         <v>393</v>
-      </c>
-      <c r="E38" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B39" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C39" t="s">
         <v>143</v>
       </c>
       <c r="D39" t="s">
+        <v>395</v>
+      </c>
+      <c r="E39" t="s">
         <v>396</v>
-      </c>
-      <c r="E39" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
+        <v>397</v>
+      </c>
+      <c r="B40" t="s">
         <v>398</v>
-      </c>
-      <c r="B40" t="s">
-        <v>399</v>
       </c>
       <c r="C40" t="s">
         <v>143</v>
       </c>
       <c r="D40" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E40" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
+        <v>400</v>
+      </c>
+      <c r="B41" t="s">
+        <v>398</v>
+      </c>
+      <c r="C41" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" t="s">
         <v>401</v>
       </c>
-      <c r="B41" t="s">
-        <v>399</v>
-      </c>
-      <c r="C41" t="s">
-        <v>142</v>
-      </c>
-      <c r="D41" t="s">
-        <v>402</v>
-      </c>
       <c r="E41" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
+        <v>404</v>
+      </c>
+      <c r="B42" t="s">
         <v>405</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
+        <v>142</v>
+      </c>
+      <c r="D42" t="s">
         <v>406</v>
       </c>
-      <c r="C42" t="s">
-        <v>142</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>407</v>
-      </c>
-      <c r="E42" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B43" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C43" t="s">
         <v>142</v>
       </c>
       <c r="D43" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E43" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B44" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C44" t="s">
         <v>143</v>
       </c>
       <c r="D44" t="s">
+        <v>410</v>
+      </c>
+      <c r="E44" t="s">
         <v>411</v>
-      </c>
-      <c r="E44" t="s">
-        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -5153,7 +5390,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5168,25 +5405,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>375</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -5202,7 +5439,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -5213,7 +5450,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -5224,7 +5461,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5235,7 +5472,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -5244,29 +5481,34 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>445</v>
+      </c>
+    </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some more cans, some weapon assets
I'm not sure if we really want melee weapons pointed off at 45 degrees like that, but that's how I did them for now. Would love some input from actual artists here. I've highlighted items that I've made on the item excel file in yellow.
</commit_message>
<xml_diff>
--- a/RPG Items.xlsx
+++ b/RPG Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ranged Weapons" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="453">
   <si>
     <t>Name</t>
   </si>
@@ -1379,6 +1379,12 @@
   </si>
   <si>
     <t>Extends the range players cal walk away from each other</t>
+  </si>
+  <si>
+    <t>machete</t>
+  </si>
+  <si>
+    <t>screwdriver</t>
   </si>
 </sst>
 </file>
@@ -1419,7 +1425,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1429,6 +1435,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1453,7 +1465,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1463,6 +1475,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1804,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2523,10 +2536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2626,7 +2639,7 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B4" t="s">
@@ -2702,7 +2715,7 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B6" t="s">
@@ -3037,7 +3050,7 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" t="s">
+      <c r="A22" s="5" t="s">
         <v>183</v>
       </c>
       <c r="B22" t="s">
@@ -3048,7 +3061,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" t="s">
+      <c r="A23" s="5" t="s">
         <v>184</v>
       </c>
       <c r="B23" t="s">
@@ -3474,6 +3487,28 @@
       </c>
       <c r="C61">
         <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="B62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>